<commit_message>
Version on the submission deadline
</commit_message>
<xml_diff>
--- a/Dataset/Captions collection/v4_test_captions_collection.xlsx
+++ b/Dataset/Captions collection/v4_test_captions_collection.xlsx
@@ -565,7 +565,7 @@
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>This graph depicts the total TKN_About in TKN_Geo in TKN_Year in cubic meters.</t>
+          <t>This graph depicts the TKN_About in TKN_Geo in TKN_Year TKN_UOM meters.</t>
         </is>
       </c>
     </row>
@@ -823,7 +823,7 @@
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>There is another high of about 57000 cubic meters in November.</t>
+          <t>There is another high of about TKN_UOM meters in November.</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>This graph depicts the total TKN_About in cubic metres of TKN_Geo in TKN_Year.</t>
+          <t>This graph depicts the TKN_About in TKN_UOM of TKN_Geo in TKN_Year.</t>
         </is>
       </c>
     </row>
@@ -995,7 +995,7 @@
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>Production starts at approximately 53000 cubic metres in January and increases to one of its maximum values of 57000 cubic metres in March.</t>
+          <t>Production starts at approximately 53000 TKN_UOM in January and increases to one of its maximum values of 57000 TKN_UOM in March.</t>
         </is>
       </c>
     </row>
@@ -1167,7 +1167,7 @@
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>From July until TKN_About gradually increases again until it reaches its second maximum of 57000 cubic metres in November.</t>
+          <t>From July until TKN_About gradually increases again until it reaches its second maximum of 57000 TKN_UOM in November.</t>
         </is>
       </c>
     </row>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>There is a sharp drop from November onwards, reaching its minimum value of 46000 cubic metres in December.</t>
+          <t>There is a sharp drop from November onwards, reaching its minimum value of 46000 TKN_UOM in December.</t>
         </is>
       </c>
     </row>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>This line graph displays total TKN_About in cubic metres in TKN_Geo for TKN_Year.</t>
+          <t>This line graph displays TKN_About in TKN_UOM in TKN_Geo for TKN_Year.</t>
         </is>
       </c>
     </row>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>A steady increase from August to November is followed by a dramatic reduction in December to a yearly low of 46000 cubic metres.</t>
+          <t>A steady increase from August to November is followed by a dramatic reduction in December to a yearly low of TKN_UOM metres.</t>
         </is>
       </c>
     </row>
@@ -1683,7 +1683,7 @@
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>The following graph shows information about the house TKN_About in TKN_Geo during TKN_Year.</t>
+          <t>The following graph shows information about TKN_About TKN_UOM in TKN_Geo during TKN_Year.</t>
         </is>
       </c>
     </row>
@@ -1769,7 +1769,7 @@
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>As can be seen from TKN_About have been steadily increasing its value over the year.</t>
+          <t>As can be seen from the graph, TKN_UOM have been steadily increasing its value over the year.</t>
         </is>
       </c>
     </row>
@@ -1941,7 +1941,7 @@
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>This graph represents the house TKN_About of TKN_Geo in TKN_Year.</t>
+          <t>This graph represents TKN_About TKN_UOM of TKN_Geo in TKN_Year.</t>
         </is>
       </c>
     </row>
@@ -2113,7 +2113,7 @@
       </c>
       <c r="X20" t="inlineStr">
         <is>
-          <t>Continuous increase of the house TKN_About in TKN_Geo during the year TKN_Year.</t>
+          <t>Continuous increase of TKN_About TKN_UOM in TKN_Geo during the year TKN_Year.</t>
         </is>
       </c>
     </row>
@@ -2199,7 +2199,7 @@
       </c>
       <c r="X21" t="inlineStr">
         <is>
-          <t>The graph shows the total TKN_About in TKN_Geo for the year TKN_Year.</t>
+          <t>The graph shows TKN_UOM in TKN_Geo for the year TKN_Year.</t>
         </is>
       </c>
     </row>
@@ -2457,7 +2457,7 @@
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>The total TKN_About from the year TKN_Year is showen by the graph.</t>
+          <t>The TKN_About from the year TKN_Year is showen by the graph.</t>
         </is>
       </c>
     </row>
@@ -2801,7 +2801,7 @@
       </c>
       <c r="X28" t="inlineStr">
         <is>
-          <t>The shown data are about the total TKN_About in TKN_Geo during TKN_Year.</t>
+          <t>The shown data are about TKN_UOM in TKN_Geo during TKN_Year.</t>
         </is>
       </c>
     </row>
@@ -3145,7 +3145,7 @@
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>Line chart showing TKN_About the Farm product price index in TKN_Geo in TKN_Year.</t>
+          <t>Line chart showing TKN_About TKN_UOM in TKN_Geo in TKN_Year.</t>
         </is>
       </c>
     </row>
@@ -3661,7 +3661,7 @@
       </c>
       <c r="X38" t="inlineStr">
         <is>
-          <t>The graph shows TKN_About fresh fruits in TKN_Geo over the year of TKN_Year.</t>
+          <t>The graph shows the TKN_About fruits in TKN_Geo over the year of TKN_Year.</t>
         </is>
       </c>
     </row>
@@ -3747,7 +3747,7 @@
       </c>
       <c r="X39" t="inlineStr">
         <is>
-          <t>In the TKN_About the year the production was nearly constant, until it fall dramatically in the mounth of August.</t>
+          <t>In the first half TKN_About was nearly constant, until it fall dramatically in the mounth of August.</t>
         </is>
       </c>
     </row>
@@ -3833,7 +3833,7 @@
       </c>
       <c r="X40" t="inlineStr">
         <is>
-          <t>Afterwards TKN_About production rises again over the index of 1100.</t>
+          <t>Afterwards the TKN_About rises again over the index of 1100.</t>
         </is>
       </c>
     </row>
@@ -3919,7 +3919,7 @@
       </c>
       <c r="X41" t="inlineStr">
         <is>
-          <t>The graph is a line chart, illustrating the commercial TKN_About in TKN_Geo.</t>
+          <t>The graph is a line chart, illustrating the TKN_About in TKN_Geo.</t>
         </is>
       </c>
     </row>
@@ -4521,7 +4521,7 @@
       </c>
       <c r="X48" t="inlineStr">
         <is>
-          <t>The commercial TKN_About in TKN_Geo considerably increased over TKN_Year.</t>
+          <t>The TKN_About in TKN_Geo considerably increased over TKN_Year.</t>
         </is>
       </c>
     </row>
@@ -4865,7 +4865,7 @@
       </c>
       <c r="X52" t="inlineStr">
         <is>
-          <t>It shows the number of TKN_About TKN_Geo during TKN_Year.</t>
+          <t>It shows the TKN_UOM of TKN_About TKN_Geo during TKN_Year.</t>
         </is>
       </c>
     </row>
@@ -5037,7 +5037,7 @@
       </c>
       <c r="X54" t="inlineStr">
         <is>
-          <t>After that, the number TKN_About TKN_Geo decrease during the last few months of the year.</t>
+          <t>After that, the TKN_UOM TKN_About TKN_Geo decrease during the last few months of the year.</t>
         </is>
       </c>
     </row>
@@ -5209,7 +5209,7 @@
       </c>
       <c r="X56" t="inlineStr">
         <is>
-          <t>The graph showes the TKN_About canada in TKN_Year.</t>
+          <t>The graph showes the TKN_About in TKN_Year.</t>
         </is>
       </c>
     </row>
@@ -5467,7 +5467,7 @@
       </c>
       <c r="X59" t="inlineStr">
         <is>
-          <t>From August till December the graph decrease continuslie till a total number of 2400000 in December.</t>
+          <t>From August till December the graph decrease continuslie TKN_About TKN_UOM of 2400000 in December.</t>
         </is>
       </c>
     </row>
@@ -5811,7 +5811,7 @@
       </c>
       <c r="X63" t="inlineStr">
         <is>
-          <t>The line chart describes the number of TKN_About TKN_Geo during TKN_Year.</t>
+          <t>The line chart describes the TKN_UOM of TKN_About TKN_Geo during TKN_Year.</t>
         </is>
       </c>
     </row>
@@ -5983,7 +5983,7 @@
       </c>
       <c r="X65" t="inlineStr">
         <is>
-          <t>During the last few months of the year the number of TKN_About TKN_Geo rapidly decreased.</t>
+          <t>During the last few months of the year the TKN_UOM of TKN_About TKN_Geo rapidly decreased.</t>
         </is>
       </c>
     </row>
@@ -6069,7 +6069,7 @@
       </c>
       <c r="X66" t="inlineStr">
         <is>
-          <t>The number TKN_About TKN_Geo during TKN_Year substantially increased over the summer months.</t>
+          <t>The TKN_UOM TKN_About TKN_Geo during TKN_Year substantially increased over the summer months.</t>
         </is>
       </c>
     </row>
@@ -6327,7 +6327,7 @@
       </c>
       <c r="X69" t="inlineStr">
         <is>
-          <t>The graph illustrates the TKN_About oats in TKN_Geo for the year TKN_Year.</t>
+          <t>The graph illustrates the TKN_About in TKN_Geo for the year TKN_Year.</t>
         </is>
       </c>
     </row>
@@ -6413,7 +6413,7 @@
       </c>
       <c r="X70" t="inlineStr">
         <is>
-          <t>There are sharp decreases in production for the TKN_About February, July and November.</t>
+          <t>There are sharp decreases in TKN_About February, July and November.</t>
         </is>
       </c>
     </row>
@@ -6499,7 +6499,7 @@
       </c>
       <c r="X71" t="inlineStr">
         <is>
-          <t>This graph shows the monthly TKN_About oats produced in TKN_Geo in TKN_Year in tonnes.</t>
+          <t>This graph shows the monthly amount TKN_About produced in TKN_Geo in TKN_Year in tonnes.</t>
         </is>
       </c>
     </row>
@@ -6585,7 +6585,7 @@
       </c>
       <c r="X72" t="inlineStr">
         <is>
-          <t>Oat production stayed within the TKN_About 80000 and 210000 tonnes each month.</t>
+          <t>Oat TKN_About 80000 and 210000 TKN_UOM each month.</t>
         </is>
       </c>
     </row>
@@ -6671,7 +6671,7 @@
       </c>
       <c r="X73" t="inlineStr">
         <is>
-          <t>While most months averaged production at around 140000 tonnes, February, June and July saw dips in production to around 90000 tonnes and the fall months saw a higher harvest, 16000 and above 200000 tonnes consecutively.</t>
+          <t>While most months TKN_About at around 140000 TKN_UOM, February, June and July saw dips in production to around 90000 TKN_UOM and the fall months saw a higher harvest, 16000 and above 200000 TKN_UOM consecutively.</t>
         </is>
       </c>
     </row>
@@ -6757,7 +6757,7 @@
       </c>
       <c r="X74" t="inlineStr">
         <is>
-          <t>The following graph depicts the Canadian TKN_About oats in tonnes during TKN_Year.</t>
+          <t>The following graph depicts the Canadian TKN_About in TKN_UOM during TKN_Year.</t>
         </is>
       </c>
     </row>
@@ -6843,7 +6843,7 @@
       </c>
       <c r="X75" t="inlineStr">
         <is>
-          <t>In January approximately 160000 tonnes were produced, after which a sharp drop can be observed for February, reaching slightly below 100000.</t>
+          <t>In January approximately 160000 TKN_UOM were produced, after which a sharp drop can be observed for February, reaching slightly below 100000.</t>
         </is>
       </c>
     </row>
@@ -7101,7 +7101,7 @@
       </c>
       <c r="X78" t="inlineStr">
         <is>
-          <t>Following this there is a drop, and production remains almost unchanged during November and December at 140000.</t>
+          <t>Following this there is a drop, TKN_About remains almost unchanged during November and December at 140000.</t>
         </is>
       </c>
     </row>
@@ -7187,7 +7187,7 @@
       </c>
       <c r="X79" t="inlineStr">
         <is>
-          <t>This graph depicts the TKN_About oats in tonnes in TKN_Geo during TKN_Year.</t>
+          <t>This graph depicts the TKN_About in TKN_UOM in TKN_Geo during TKN_Year.</t>
         </is>
       </c>
     </row>
@@ -7359,7 +7359,7 @@
       </c>
       <c r="X81" t="inlineStr">
         <is>
-          <t>For the following months production slightly increases until August.</t>
+          <t>For the following TKN_About slightly increases until August.</t>
         </is>
       </c>
     </row>
@@ -7445,7 +7445,7 @@
       </c>
       <c r="X82" t="inlineStr">
         <is>
-          <t>Between August and September a rapid increase in production can be observed, indicating the TKN_About over 200000 in September.</t>
+          <t>Between August and September a rapid increase TKN_About can be observed, indicating the maximum of over 200000 in September.</t>
         </is>
       </c>
     </row>
@@ -7617,7 +7617,7 @@
       </c>
       <c r="X84" t="inlineStr">
         <is>
-          <t>The TKN_About oats strongly fluctuated over the TKN_Year in TKN_Geo.</t>
+          <t>The TKN_About strongly fluctuated over the TKN_Year in TKN_Geo.</t>
         </is>
       </c>
     </row>
@@ -7961,7 +7961,7 @@
       </c>
       <c r="X88" t="inlineStr">
         <is>
-          <t>The figure shows a line chart about the production TKN_About (in tonnes) in TKN_Geo during TKN_Year.</t>
+          <t>The figure shows a line chart about the TKN_About (in tonnes) in TKN_Geo during TKN_Year.</t>
         </is>
       </c>
     </row>
@@ -8133,7 +8133,7 @@
       </c>
       <c r="X90" t="inlineStr">
         <is>
-          <t>Even that, if it has been recorded a significant growth from November to December, where the production TKN_About during TKN_Year reached its peak.</t>
+          <t>Even that, if it has been recorded a significant growth from November to December, where the TKN_About during TKN_Year reached its peak.</t>
         </is>
       </c>
     </row>
@@ -8219,7 +8219,7 @@
       </c>
       <c r="X91" t="inlineStr">
         <is>
-          <t>The graph shows the production TKN_About in tonnes in TKN_Geo in TKN_Year.</t>
+          <t>The graph shows the TKN_About in TKN_UOM in TKN_Geo in TKN_Year.</t>
         </is>
       </c>
     </row>
@@ -8735,7 +8735,7 @@
       </c>
       <c r="X97" t="inlineStr">
         <is>
-          <t>The line chart is displaying the recorded data about production TKN_About in TKN_Geo during TKN_Year.</t>
+          <t>The line chart is displaying the recorded data about TKN_About in TKN_Geo during TKN_Year.</t>
         </is>
       </c>
     </row>
@@ -8821,7 +8821,7 @@
       </c>
       <c r="X98" t="inlineStr">
         <is>
-          <t>The TKN_About production have been recorded during the months of January, August and November.</t>
+          <t>The minimum TKN_About have been recorded during the months of January, August and November.</t>
         </is>
       </c>
     </row>
@@ -8993,7 +8993,7 @@
       </c>
       <c r="X100" t="inlineStr">
         <is>
-          <t>The TKN_About production over the year was recorded during December.</t>
+          <t>The maximum TKN_About over the year was recorded during December.</t>
         </is>
       </c>
     </row>
@@ -9079,7 +9079,7 @@
       </c>
       <c r="X101" t="inlineStr">
         <is>
-          <t>This graph represents the production TKN_About in TKN_Geo in TKN_Year (in tonnes).</t>
+          <t>This graph represents the TKN_About in TKN_Geo in TKN_Year (in tonnes).</t>
         </is>
       </c>
     </row>
@@ -9251,7 +9251,7 @@
       </c>
       <c r="X103" t="inlineStr">
         <is>
-          <t>There is a sharp increase during February and during the following months production levels off between 29000 and 32500.</t>
+          <t>There is a sharp increase during February and during the TKN_About levels off between 29000 and 32500.</t>
         </is>
       </c>
     </row>
@@ -9423,7 +9423,7 @@
       </c>
       <c r="X105" t="inlineStr">
         <is>
-          <t>For the following 2 months production TKN_About remains steady at approximately 30000.</t>
+          <t>For the following 2 months TKN_About remains steady at approximately 30000.</t>
         </is>
       </c>
     </row>
@@ -9509,7 +9509,7 @@
       </c>
       <c r="X106" t="inlineStr">
         <is>
-          <t>After a drop in November, production peaks in December with up to 40000 tonnes.</t>
+          <t>After a drop TKN_About peaks in December with up to 40000 tonnes.</t>
         </is>
       </c>
     </row>

</xml_diff>